<commit_message>
Jan 7 - CXT Run input
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CXTValidation/cxt_runinput.xlsx
+++ b/gr/Input_Output/CXTValidation/cxt_runinput.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bharathi\git\gr\gr\Input_Output\CXTValidation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Git\gr\gr\Input_Output\CXTValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBE7159-69C4-4090-9EEC-57021BC4183A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rundata" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="19">
   <si>
     <t>Environment</t>
   </si>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,7 +155,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -466,23 +467,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -516,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -533,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -550,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -561,13 +562,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -584,12 +585,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -601,12 +602,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -618,25 +619,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -656,22 +640,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -705,7 +689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -722,7 +706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -739,17 +723,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -766,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -783,7 +767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -800,12 +784,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -822,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updating run input file
</commit_message>
<xml_diff>
--- a/gr/Input_Output/CXTValidation/cxt_runinput.xlsx
+++ b/gr/Input_Output/CXTValidation/cxt_runinput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Git\gr\gr\Input_Output\CXTValidation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Code\gr-master\gr\Input_Output\CXTValidation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBE7159-69C4-4090-9EEC-57021BC4183A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4511AE5F-59F7-4383-9313-5618A6E4184B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rundata" sheetId="1" r:id="rId1"/>
@@ -471,19 +471,19 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -517,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -534,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -551,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -568,7 +568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -585,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -602,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -619,7 +619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -647,15 +647,15 @@
       <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -689,7 +689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -706,7 +706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -723,17 +723,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -750,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -767,7 +767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -784,12 +784,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -806,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>6</v>
       </c>

</xml_diff>